<commit_message>
update balance function added
</commit_message>
<xml_diff>
--- a/balances/balances.xlsx
+++ b/balances/balances.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabe/go/src/github.com/Gabe1203/Finances/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E91830-816D-7E4B-A04F-C32B5FCFA56E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15960" xr2:uid="{2E9F8BCA-09A8-EB40-9F6B-5C44EA85C703}"/>
+    <workbookView windowHeight="15960" windowWidth="27640" xWindow="780" yWindow="940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,10 +63,16 @@
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -173,26 +173,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -500,34 +500,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7260FD72-CEC8-4841-A436-88A715833F0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="42.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="2" spans="1:2" thickBot="true">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row ht="17" r="3" spans="1:2" thickBot="true">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="4" spans="1:2" thickBot="true">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="5" spans="1:2" thickBot="true">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -551,7 +551,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="6" spans="1:2" thickBot="true">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -559,7 +559,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="7" spans="1:2" thickBot="true">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -572,6 +572,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>